<commit_message>
Automatic update of files.
</commit_message>
<xml_diff>
--- a/Logging_BLEKINGE_LAN/Logging_KARLSHAMN/Översikt KARLSHAMN.xlsx
+++ b/Logging_BLEKINGE_LAN/Logging_KARLSHAMN/Översikt KARLSHAMN.xlsx
@@ -572,7 +572,7 @@
         <v>45108</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>45170</v>
+        <v>45174</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -629,7 +629,7 @@
         <v>45114</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>45170</v>
+        <v>45174</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -686,7 +686,7 @@
         <v>45114</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>45170</v>
+        <v>45174</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -743,7 +743,7 @@
         <v>45117</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>45170</v>
+        <v>45174</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -800,7 +800,7 @@
         <v>45118</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>45170</v>
+        <v>45174</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -857,7 +857,7 @@
         <v>45118</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>45170</v>
+        <v>45174</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -914,7 +914,7 @@
         <v>45118</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>45170</v>
+        <v>45174</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -971,7 +971,7 @@
         <v>45118</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>45170</v>
+        <v>45174</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
         <v>45119</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>45170</v>
+        <v>45174</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1085,7 +1085,7 @@
         <v>45119</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>45170</v>
+        <v>45174</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>

</xml_diff>